<commit_message>
some more testing and fixes
</commit_message>
<xml_diff>
--- a/MonteCarloResultsBUS6Sub2MLoadCurve.xlsx
+++ b/MonteCarloResultsBUS6Sub2MLoadCurve.xlsx
@@ -148,10 +148,10 @@
     <t>farm</t>
   </si>
   <si>
-    <t>(40.674686364284554, 44.00977880916459)</t>
-  </si>
-  <si>
-    <t>(40.150600408660544, 44.533864764788596)</t>
+    <t>(40.99696059205935, 44.27060488485948)</t>
+  </si>
+  <si>
+    <t>(40.482530774619335, 44.7850347022995)</t>
   </si>
 </sst>
 </file>
@@ -588,28 +588,28 @@
         <v>147</v>
       </c>
       <c r="F2">
-        <v>7.339801560973719</v>
+        <v>7.154416604221201</v>
       </c>
       <c r="G2">
-        <v>3188</v>
+        <v>3368</v>
       </c>
       <c r="H2">
-        <v>5.564711534778382</v>
+        <v>5.533626856887242</v>
       </c>
       <c r="I2">
-        <v>1.318990484071163</v>
+        <v>1.292898272552783</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
       <c r="K2">
-        <v>193.8916011584609</v>
+        <v>190.0560460652591</v>
       </c>
       <c r="L2">
-        <v>1078.950829463137</v>
+        <v>1051.699240820517</v>
       </c>
       <c r="M2">
-        <v>818.012595612422</v>
+        <v>813.4431479624245</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -629,28 +629,28 @@
         <v>126</v>
       </c>
       <c r="F3">
-        <v>7.229721844511835</v>
+        <v>7.162775857171653</v>
       </c>
       <c r="G3">
-        <v>3179</v>
+        <v>3370</v>
       </c>
       <c r="H3">
-        <v>5.496771845921707</v>
+        <v>5.536804483065922</v>
       </c>
       <c r="I3">
-        <v>1.315266859743484</v>
+        <v>1.293666026871401</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
       <c r="K3">
-        <v>165.7236243276789</v>
+        <v>163.0019193857965</v>
       </c>
       <c r="L3">
-        <v>910.9449524084912</v>
+        <v>902.5097580036282</v>
       </c>
       <c r="M3">
-        <v>692.593252586135</v>
+        <v>697.6373648663061</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -670,28 +670,28 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>7.230760803124549</v>
+        <v>7.227408007736686</v>
       </c>
       <c r="G4">
-        <v>3183</v>
+        <v>3373</v>
       </c>
       <c r="H4">
-        <v>5.490653113776951</v>
+        <v>5.581795985815021</v>
       </c>
       <c r="I4">
-        <v>1.316921803889119</v>
+        <v>1.294817658349328</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4">
-        <v>1.316921803889119</v>
+        <v>1.294817658349328</v>
       </c>
       <c r="L4">
-        <v>7.230760803124549</v>
+        <v>7.227408007736686</v>
       </c>
       <c r="M4">
-        <v>5.490653113776951</v>
+        <v>5.581795985815021</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -711,28 +711,28 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <v>7.234056774398391</v>
+        <v>7.128121435560409</v>
       </c>
       <c r="G5">
-        <v>3182</v>
+        <v>3361</v>
       </c>
       <c r="H5">
-        <v>5.494882219899721</v>
+        <v>5.524771300099633</v>
       </c>
       <c r="I5">
-        <v>1.31650806785271</v>
+        <v>1.29021113243762</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
       <c r="K5">
-        <v>1.31650806785271</v>
+        <v>1.29021113243762</v>
       </c>
       <c r="L5">
-        <v>7.234056774398391</v>
+        <v>7.128121435560409</v>
       </c>
       <c r="M5">
-        <v>5.494882219899721</v>
+        <v>5.524771300099633</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -752,28 +752,28 @@
         <v>132</v>
       </c>
       <c r="F6">
-        <v>8.614587304936117</v>
+        <v>8.576099391575989</v>
       </c>
       <c r="G6">
-        <v>3185</v>
+        <v>3361</v>
       </c>
       <c r="H6">
-        <v>6.537349298596734</v>
+        <v>6.647051149971869</v>
       </c>
       <c r="I6">
-        <v>1.317749275961936</v>
+        <v>1.29021113243762</v>
       </c>
       <c r="J6">
         <v>0</v>
       </c>
       <c r="K6">
-        <v>173.9429044269756</v>
+        <v>170.3078694817658</v>
       </c>
       <c r="L6">
-        <v>1137.125524251567</v>
+        <v>1132.045119688031</v>
       </c>
       <c r="M6">
-        <v>862.9301074147688</v>
+        <v>877.4107517962867</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -793,28 +793,28 @@
         <v>147</v>
       </c>
       <c r="F7">
-        <v>8.954427281265856</v>
+        <v>8.70404732026708</v>
       </c>
       <c r="G7">
-        <v>3268</v>
+        <v>3425</v>
       </c>
       <c r="H7">
-        <v>6.622659344804031</v>
+        <v>6.620158618772479</v>
       </c>
       <c r="I7">
-        <v>1.352089366983864</v>
+        <v>1.314779270633397</v>
       </c>
       <c r="J7">
         <v>0</v>
       </c>
       <c r="K7">
-        <v>198.757136946628</v>
+        <v>193.2725527831094</v>
       </c>
       <c r="L7">
-        <v>1316.300810346081</v>
+        <v>1279.494956079261</v>
       </c>
       <c r="M7">
-        <v>973.5309236861926</v>
+        <v>973.1633169595544</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -834,28 +834,28 @@
         <v>1</v>
       </c>
       <c r="F8">
-        <v>8.927108369403621</v>
+        <v>8.844535439013768</v>
       </c>
       <c r="G8">
-        <v>3256</v>
+        <v>3460</v>
       </c>
       <c r="H8">
-        <v>6.626787754560366</v>
+        <v>6.658963820413545</v>
       </c>
       <c r="I8">
-        <v>1.347124534546959</v>
+        <v>1.328214971209213</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
       <c r="K8">
-        <v>1.347124534546959</v>
+        <v>1.328214971209213</v>
       </c>
       <c r="L8">
-        <v>8.927108369403621</v>
+        <v>8.844535439013768</v>
       </c>
       <c r="M8">
-        <v>6.626787754560366</v>
+        <v>6.658963820413545</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -875,28 +875,28 @@
         <v>79</v>
       </c>
       <c r="F9">
-        <v>8.727327211023148</v>
+        <v>8.562837106637131</v>
       </c>
       <c r="G9">
-        <v>3192</v>
+        <v>3370</v>
       </c>
       <c r="H9">
-        <v>6.608380284787891</v>
+        <v>6.619047674418317</v>
       </c>
       <c r="I9">
-        <v>1.320645428216798</v>
+        <v>1.293666026871401</v>
       </c>
       <c r="J9">
         <v>0</v>
       </c>
       <c r="K9">
-        <v>104.330988829127</v>
+        <v>102.1996161228407</v>
       </c>
       <c r="L9">
-        <v>689.4588496708287</v>
+        <v>676.4641314243333</v>
       </c>
       <c r="M9">
-        <v>522.0620424982434</v>
+        <v>522.9047662790471</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -916,28 +916,28 @@
         <v>1</v>
       </c>
       <c r="F10">
-        <v>10.60995150262355</v>
+        <v>10.96173286320302</v>
       </c>
       <c r="G10">
-        <v>3236</v>
+        <v>3434</v>
       </c>
       <c r="H10">
-        <v>7.924676384994163</v>
+        <v>8.315467125405904</v>
       </c>
       <c r="I10">
-        <v>1.338849813818784</v>
+        <v>1.318234165067178</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10">
-        <v>1.338849813818784</v>
+        <v>1.318234165067178</v>
       </c>
       <c r="L10">
-        <v>10.60995150262355</v>
+        <v>10.96173286320302</v>
       </c>
       <c r="M10">
-        <v>7.924676384994163</v>
+        <v>8.315467125405904</v>
       </c>
     </row>
     <row r="11" spans="1:19">
@@ -957,28 +957,28 @@
         <v>76</v>
       </c>
       <c r="F11">
-        <v>10.51061301226996</v>
+        <v>10.75001749080373</v>
       </c>
       <c r="G11">
-        <v>3188</v>
+        <v>3363</v>
       </c>
       <c r="H11">
-        <v>7.968679940607428</v>
+        <v>8.327028118805744</v>
       </c>
       <c r="I11">
-        <v>1.318990484071163</v>
+        <v>1.290978886756238</v>
       </c>
       <c r="J11">
         <v>0</v>
       </c>
       <c r="K11">
-        <v>100.2432767894084</v>
+        <v>98.11439539347408</v>
       </c>
       <c r="L11">
-        <v>798.8065889325165</v>
+        <v>817.0013293010835</v>
       </c>
       <c r="M11">
-        <v>605.6196754861645</v>
+        <v>632.8541370292365</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -998,28 +998,28 @@
         <v>79</v>
       </c>
       <c r="F12">
-        <v>11.63464496218396</v>
+        <v>12.13853046600683</v>
       </c>
       <c r="G12">
-        <v>3532</v>
+        <v>3761</v>
       </c>
       <c r="H12">
-        <v>7.961760156738007</v>
+        <v>8.407570290866202</v>
       </c>
       <c r="I12">
-        <v>1.46131568059578</v>
+        <v>1.443761996161228</v>
       </c>
       <c r="J12">
         <v>0</v>
       </c>
       <c r="K12">
-        <v>115.4439387670666</v>
+        <v>114.057197696737</v>
       </c>
       <c r="L12">
-        <v>919.136952012533</v>
+        <v>958.9439068145394</v>
       </c>
       <c r="M12">
-        <v>628.9790523823025</v>
+        <v>664.1980529784299</v>
       </c>
     </row>
     <row r="13" spans="1:19">
@@ -1039,28 +1039,28 @@
         <v>76</v>
       </c>
       <c r="F13">
-        <v>11.70447565152951</v>
+        <v>12.08417892488875</v>
       </c>
       <c r="G13">
-        <v>3537</v>
+        <v>3765</v>
       </c>
       <c r="H13">
-        <v>7.998223819549567</v>
+        <v>8.361032164498058</v>
       </c>
       <c r="I13">
-        <v>1.463384360777824</v>
+        <v>1.445297504798464</v>
       </c>
       <c r="J13">
         <v>0</v>
       </c>
       <c r="K13">
-        <v>111.2172114191146</v>
+        <v>109.8426103646833</v>
       </c>
       <c r="L13">
-        <v>889.5401495162426</v>
+        <v>918.3975982915447</v>
       </c>
       <c r="M13">
-        <v>607.8650102857671</v>
+        <v>635.4384445018524</v>
       </c>
     </row>
     <row r="14" spans="1:19">
@@ -1080,28 +1080,28 @@
         <v>1</v>
       </c>
       <c r="F14">
-        <v>12.50755908777945</v>
+        <v>13.07908221836684</v>
       </c>
       <c r="G14">
-        <v>3801</v>
+        <v>4080</v>
       </c>
       <c r="H14">
-        <v>7.953372879548258</v>
+        <v>8.350737543834711</v>
       </c>
       <c r="I14">
-        <v>1.572610674389739</v>
+        <v>1.566218809980806</v>
       </c>
       <c r="J14">
         <v>0</v>
       </c>
       <c r="K14">
-        <v>1.572610674389739</v>
+        <v>1.566218809980806</v>
       </c>
       <c r="L14">
-        <v>12.50755908777945</v>
+        <v>13.07908221836684</v>
       </c>
       <c r="M14">
-        <v>7.953372879548258</v>
+        <v>8.350737543834711</v>
       </c>
     </row>
     <row r="15" spans="1:19">
@@ -1121,28 +1121,28 @@
         <v>79</v>
       </c>
       <c r="F15">
-        <v>11.15195265354554</v>
+        <v>11.21469154759746</v>
       </c>
       <c r="G15">
-        <v>3940</v>
+        <v>4185</v>
       </c>
       <c r="H15">
-        <v>6.841185168431363</v>
+        <v>6.980710031419688</v>
       </c>
       <c r="I15">
-        <v>1.630119983450559</v>
+        <v>1.606525911708253</v>
       </c>
       <c r="J15">
         <v>0</v>
       </c>
       <c r="K15">
-        <v>128.7794786925941</v>
+        <v>126.915547024952</v>
       </c>
       <c r="L15">
-        <v>881.0042596300977</v>
+        <v>885.9606322601996</v>
       </c>
       <c r="M15">
-        <v>540.4536283060777</v>
+        <v>551.4760924821554</v>
       </c>
     </row>
     <row r="16" spans="1:19">
@@ -1162,28 +1162,28 @@
         <v>1</v>
       </c>
       <c r="F16">
-        <v>11.40237338003394</v>
+        <v>11.58012555269163</v>
       </c>
       <c r="G16">
-        <v>4013</v>
+        <v>4300</v>
       </c>
       <c r="H16">
-        <v>6.867564530162478</v>
+        <v>7.015401642967836</v>
       </c>
       <c r="I16">
-        <v>1.660322714108399</v>
+        <v>1.650671785028791</v>
       </c>
       <c r="J16">
         <v>0</v>
       </c>
       <c r="K16">
-        <v>1.660322714108399</v>
+        <v>1.650671785028791</v>
       </c>
       <c r="L16">
-        <v>11.40237338003394</v>
+        <v>11.58012555269163</v>
       </c>
       <c r="M16">
-        <v>6.867564530162478</v>
+        <v>7.015401642967836</v>
       </c>
     </row>
     <row r="17" spans="1:19">
@@ -1203,28 +1203,28 @@
         <v>76</v>
       </c>
       <c r="F17">
-        <v>11.19500481051688</v>
+        <v>11.20225482720165</v>
       </c>
       <c r="G17">
-        <v>3942</v>
+        <v>4182</v>
       </c>
       <c r="H17">
-        <v>6.864111270172321</v>
+        <v>6.977970785475918</v>
       </c>
       <c r="I17">
-        <v>1.630947455523376</v>
+        <v>1.605374280230326</v>
       </c>
       <c r="J17">
         <v>0</v>
       </c>
       <c r="K17">
-        <v>123.9520066197766</v>
+        <v>122.0084452975048</v>
       </c>
       <c r="L17">
-        <v>850.8203655992826</v>
+        <v>851.3713668673253</v>
       </c>
       <c r="M17">
-        <v>521.6724565330965</v>
+        <v>530.3257796961698</v>
       </c>
     </row>
     <row r="18" spans="1:19">
@@ -1244,28 +1244,28 @@
         <v>1</v>
       </c>
       <c r="F18">
-        <v>11.25741349001558</v>
+        <v>11.20810775522187</v>
       </c>
       <c r="G18">
-        <v>3946</v>
+        <v>4188</v>
       </c>
       <c r="H18">
-        <v>6.895379727665397</v>
+        <v>6.971614303331652</v>
       </c>
       <c r="I18">
-        <v>1.632602399669011</v>
+        <v>1.607677543186181</v>
       </c>
       <c r="J18">
         <v>0</v>
       </c>
       <c r="K18">
-        <v>1.632602399669011</v>
+        <v>1.607677543186181</v>
       </c>
       <c r="L18">
-        <v>11.25741349001558</v>
+        <v>11.20810775522187</v>
       </c>
       <c r="M18">
-        <v>6.895379727665397</v>
+        <v>6.971614303331652</v>
       </c>
     </row>
     <row r="19" spans="1:19">
@@ -1285,28 +1285,28 @@
         <v>1</v>
       </c>
       <c r="F19">
-        <v>12.39843685289851</v>
+        <v>12.3437948278395</v>
       </c>
       <c r="G19">
-        <v>4298</v>
+        <v>4566</v>
       </c>
       <c r="H19">
-        <v>6.972317792800302</v>
+        <v>7.0423971805786</v>
       </c>
       <c r="I19">
-        <v>1.778237484484899</v>
+        <v>1.75278310940499</v>
       </c>
       <c r="J19">
         <v>0</v>
       </c>
       <c r="K19">
-        <v>1.778237484484899</v>
+        <v>1.75278310940499</v>
       </c>
       <c r="L19">
-        <v>12.39843685289851</v>
+        <v>12.3437948278395</v>
       </c>
       <c r="M19">
-        <v>6.972317792800302</v>
+        <v>7.0423971805786</v>
       </c>
     </row>
     <row r="20" spans="1:19">
@@ -1326,28 +1326,28 @@
         <v>79</v>
       </c>
       <c r="F20">
-        <v>13.28985556842857</v>
+        <v>13.63133984295464</v>
       </c>
       <c r="G20">
-        <v>3982</v>
+        <v>4275</v>
       </c>
       <c r="H20">
-        <v>8.066695356326434</v>
+        <v>8.306348606057739</v>
       </c>
       <c r="I20">
-        <v>1.647496896979727</v>
+        <v>1.641074856046065</v>
       </c>
       <c r="J20">
         <v>0</v>
       </c>
       <c r="K20">
-        <v>130.1522548613984</v>
+        <v>129.6449136276392</v>
       </c>
       <c r="L20">
-        <v>1049.898589905857</v>
+        <v>1076.875847593417</v>
       </c>
       <c r="M20">
-        <v>637.2689331497883</v>
+        <v>656.2015398785613</v>
       </c>
     </row>
     <row r="21" spans="1:19">
@@ -1367,28 +1367,28 @@
         <v>1</v>
       </c>
       <c r="F21">
-        <v>13.39795400045528</v>
+        <v>13.98522409002334</v>
       </c>
       <c r="G21">
-        <v>4059</v>
+        <v>4373</v>
       </c>
       <c r="H21">
-        <v>7.978037649445779</v>
+        <v>8.331010462956966</v>
       </c>
       <c r="I21">
-        <v>1.679354571783202</v>
+        <v>1.678694817658349</v>
       </c>
       <c r="J21">
         <v>0</v>
       </c>
       <c r="K21">
-        <v>1.679354571783202</v>
+        <v>1.678694817658349</v>
       </c>
       <c r="L21">
-        <v>13.39795400045528</v>
+        <v>13.98522409002334</v>
       </c>
       <c r="M21">
-        <v>7.978037649445779</v>
+        <v>8.331010462956966</v>
       </c>
     </row>
     <row r="22" spans="1:19">
@@ -1408,28 +1408,28 @@
         <v>1</v>
       </c>
       <c r="F22">
-        <v>13.14588525187122</v>
+        <v>13.79522922811361</v>
       </c>
       <c r="G22">
-        <v>3976</v>
+        <v>4284</v>
       </c>
       <c r="H22">
-        <v>7.99134925899717</v>
+        <v>8.388555588056947</v>
       </c>
       <c r="I22">
-        <v>1.645014480761274</v>
+        <v>1.644529750479846</v>
       </c>
       <c r="J22">
         <v>0</v>
       </c>
       <c r="K22">
-        <v>1.645014480761274</v>
+        <v>1.644529750479846</v>
       </c>
       <c r="L22">
-        <v>13.14588525187122</v>
+        <v>13.79522922811361</v>
       </c>
       <c r="M22">
-        <v>7.99134925899717</v>
+        <v>8.388555588056947</v>
       </c>
     </row>
     <row r="23" spans="1:19">
@@ -1449,28 +1449,28 @@
         <v>76</v>
       </c>
       <c r="F23">
-        <v>13.1467899459398</v>
+        <v>13.79137052491314</v>
       </c>
       <c r="G23">
-        <v>3973</v>
+        <v>4289</v>
       </c>
       <c r="H23">
-        <v>7.997933878514096</v>
+        <v>8.376432785590751</v>
       </c>
       <c r="I23">
-        <v>1.643773272652048</v>
+        <v>1.646449136276392</v>
       </c>
       <c r="J23">
         <v>0</v>
       </c>
       <c r="K23">
-        <v>124.9267687215556</v>
+        <v>125.1301343570058</v>
       </c>
       <c r="L23">
-        <v>999.1560358914251</v>
+        <v>1048.144159893399</v>
       </c>
       <c r="M23">
-        <v>607.8429747670713</v>
+        <v>636.6088917048971</v>
       </c>
     </row>
     <row r="24" spans="1:19">
@@ -1490,28 +1490,28 @@
         <v>1</v>
       </c>
       <c r="F24">
-        <v>14.16366267792653</v>
+        <v>14.67455481283108</v>
       </c>
       <c r="G24">
-        <v>4263</v>
+        <v>4622</v>
       </c>
       <c r="H24">
-        <v>8.030394720278773</v>
+        <v>8.270708629905878</v>
       </c>
       <c r="I24">
-        <v>1.763756723210592</v>
+        <v>1.774280230326296</v>
       </c>
       <c r="J24">
         <v>0</v>
       </c>
       <c r="K24">
-        <v>1.763756723210592</v>
+        <v>1.774280230326296</v>
       </c>
       <c r="L24">
-        <v>14.16366267792653</v>
+        <v>14.67455481283108</v>
       </c>
       <c r="M24">
-        <v>8.030394720278773</v>
+        <v>8.270708629905878</v>
       </c>
     </row>
     <row r="25" spans="1:19">
@@ -1528,25 +1528,25 @@
         <v>1183</v>
       </c>
       <c r="K25">
-        <v>1.42722949689628</v>
+        <v>1.404444278591628</v>
       </c>
       <c r="L25">
-        <v>9.842281546761278</v>
+        <v>9.910174102508774</v>
       </c>
       <c r="M25">
-        <v>6.896074925696785</v>
+        <v>7.056295684757719</v>
       </c>
       <c r="N25">
-        <v>42.34223258672456</v>
+        <v>42.6337827384594</v>
       </c>
       <c r="O25">
-        <v>2417</v>
+        <v>2605</v>
       </c>
       <c r="P25">
         <v>0.02</v>
       </c>
       <c r="Q25">
-        <v>0.02009315137687742</v>
+        <v>0.01958806576285069</v>
       </c>
       <c r="R25" t="s">
         <v>44</v>

</xml_diff>